<commit_message>
Corrections check list log
</commit_message>
<xml_diff>
--- a/6_Valkyriz/Direction logistique/Checklist logistique.xlsx
+++ b/6_Valkyriz/Direction logistique/Checklist logistique.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Test-Data\6_Valkyriz\Direction logistique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461993C8-F103-469D-B368-D0844EC89625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD34222-8930-427C-9D10-2C0F9F025602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15216" yWindow="4524" windowWidth="23040" windowHeight="10884" xr2:uid="{628984AC-6DD3-4E6D-B663-80382EC75214}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{628984AC-6DD3-4E6D-B663-80382EC75214}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -180,9 +180,6 @@
     <t>Pyromètre</t>
   </si>
   <si>
-    <t>Mètres 2m et 30m</t>
-  </si>
-  <si>
     <t>Décamètre</t>
   </si>
   <si>
@@ -411,7 +408,10 @@
     <t>Roues</t>
   </si>
   <si>
-    <t>Remorques</t>
+    <t xml:space="preserve">Mètres </t>
+  </si>
+  <si>
+    <t>Remorque</t>
   </si>
 </sst>
 </file>
@@ -516,8 +516,20 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -526,18 +538,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5950,8 +5950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B747EE-2C87-45B3-AA3E-B24141D9260C}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5963,288 +5963,288 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7" t="s">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="7" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7" t="s">
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="7" t="s">
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="7" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="7" t="s">
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="7" t="s">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -6274,36 +6274,36 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="G30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" t="s">
         <v>53</v>
-      </c>
-      <c r="G34" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G35" t="s">
         <v>37</v>
@@ -6311,277 +6311,277 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
+        <v>55</v>
+      </c>
+      <c r="G36" t="s">
         <v>56</v>
-      </c>
-      <c r="G36" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" t="s">
         <v>58</v>
-      </c>
-      <c r="G37" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
+        <v>59</v>
+      </c>
+      <c r="G38" t="s">
         <v>60</v>
-      </c>
-      <c r="G38" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
+        <v>62</v>
+      </c>
+      <c r="G39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="C41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" t="s">
         <v>65</v>
-      </c>
-      <c r="G42" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
+        <v>68</v>
+      </c>
+      <c r="G44" t="s">
         <v>69</v>
-      </c>
-      <c r="G44" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
+        <v>70</v>
+      </c>
+      <c r="G45" t="s">
         <v>71</v>
-      </c>
-      <c r="G45" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
+        <v>74</v>
+      </c>
+      <c r="G47" t="s">
         <v>75</v>
       </c>
-      <c r="G47" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>78</v>
+      <c r="A48" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
+        <v>78</v>
+      </c>
+      <c r="G49" t="s">
         <v>79</v>
-      </c>
-      <c r="G49" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
+        <v>80</v>
+      </c>
+      <c r="G50" t="s">
         <v>81</v>
-      </c>
-      <c r="G50" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
+        <v>82</v>
+      </c>
+      <c r="G51" t="s">
         <v>83</v>
-      </c>
-      <c r="G51" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
+        <v>84</v>
+      </c>
+      <c r="G52" t="s">
         <v>85</v>
-      </c>
-      <c r="G52" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
+        <v>86</v>
+      </c>
+      <c r="G53" t="s">
         <v>87</v>
-      </c>
-      <c r="G53" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
+        <v>88</v>
+      </c>
+      <c r="G54" t="s">
         <v>89</v>
-      </c>
-      <c r="G54" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
+        <v>90</v>
+      </c>
+      <c r="G55" t="s">
         <v>91</v>
-      </c>
-      <c r="G55" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
+        <v>92</v>
+      </c>
+      <c r="G56" t="s">
         <v>93</v>
-      </c>
-      <c r="G56" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
+        <v>95</v>
+      </c>
+      <c r="G57" t="s">
         <v>96</v>
-      </c>
-      <c r="G57" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
+        <v>97</v>
+      </c>
+      <c r="G58" t="s">
         <v>98</v>
-      </c>
-      <c r="G58" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
+        <v>99</v>
+      </c>
+      <c r="G59" t="s">
         <v>100</v>
-      </c>
-      <c r="G59" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>102</v>
+      <c r="A62" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
+        <v>102</v>
+      </c>
+      <c r="G63" t="s">
         <v>103</v>
-      </c>
-      <c r="G63" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
+        <v>104</v>
+      </c>
+      <c r="G64" t="s">
         <v>105</v>
-      </c>
-      <c r="G64" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
+        <v>106</v>
+      </c>
+      <c r="G65" t="s">
         <v>107</v>
-      </c>
-      <c r="G65" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C66" t="s">
+        <v>108</v>
+      </c>
+      <c r="G66" t="s">
         <v>109</v>
-      </c>
-      <c r="G66" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
+        <v>110</v>
+      </c>
+      <c r="G67" t="s">
         <v>111</v>
-      </c>
-      <c r="G67" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
+        <v>112</v>
+      </c>
+      <c r="G68" t="s">
         <v>113</v>
-      </c>
-      <c r="G68" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
+        <v>116</v>
+      </c>
+      <c r="G72" t="s">
         <v>117</v>
-      </c>
-      <c r="G72" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
+        <v>118</v>
+      </c>
+      <c r="G73" t="s">
         <v>119</v>
-      </c>
-      <c r="G73" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C74" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -6589,29 +6589,35 @@
         <v>125</v>
       </c>
       <c r="G77" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C78" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="85" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F85" s="2"/>
+      <c r="F85" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
     <mergeCell ref="G16:I16"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="C23:E23"/>
@@ -6628,32 +6634,26 @@
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="G21:I21"/>
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="G19:I19"/>
     <mergeCell ref="G18:I18"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D4:G4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;C&amp;"-,Gras"&amp;18&amp;KFF0000Check-list Logistique&amp;R&amp;G
 </oddHeader>
-    <oddFooter>&amp;LPar RCT&amp;CVersion 4.1&amp;RTest-data-&gt;6</oddFooter>
+    <oddFooter>&amp;LPar RCT&amp;CVersion 4.1 01/10/2020&amp;RTest-data-&gt;6</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <legacyDrawingHF r:id="rId3"/>

</xml_diff>